<commit_message>
Added SMS Sender for repair
</commit_message>
<xml_diff>
--- a/Templates/Repair_history.xlsx
+++ b/Templates/Repair_history.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,12 +446,11 @@
   <cols>
     <col min="1" max="1" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="11" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="5" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" style="5" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>